<commit_message>
Changes to read data from Excel and added log4j files
</commit_message>
<xml_diff>
--- a/DSAlgoPortal/src/test/resources/ExcelTestData/LoginData.xlsx
+++ b/DSAlgoPortal/src/test/resources/ExcelTestData/LoginData.xlsx
@@ -3,19 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac2a94ecd36d7ac4/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{92171399-D285-4434-92A2-0BF22FC3E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DC2CB70-9EA7-423A-B2B3-75CF6ED05A97}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5BFCB8F7-ED19-43F0-8CC2-820C6282730F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="register" sheetId="2" r:id="rId2"/>
+    <sheet name="tryEditor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:H23"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -58,6 +56,45 @@
   </si>
   <si>
     <t>Time2fly$1</t>
+  </si>
+  <si>
+    <t>password confirmation</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>Time2fly</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>techtitanstest</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as</t>
+  </si>
+  <si>
+    <t>python code</t>
+  </si>
+  <si>
+    <t>alert message</t>
+  </si>
+  <si>
+    <t>print"hello"</t>
+  </si>
+  <si>
+    <t>print"hello";;</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>techtitanstest4</t>
   </si>
 </sst>
 </file>
@@ -81,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,13 +141,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,4 +536,246 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45CE0B8-E5BE-428F-B2FF-16A458B34D63}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12345678901</v>
+      </c>
+      <c r="C9" s="3">
+        <v>12345678901</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4070884-C656-4598-9D98-EC54A4CE7753}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>